<commit_message>
staff logout and dashboard name
</commit_message>
<xml_diff>
--- a/F21MP/Testing/Student Testing/Survey Results/Post-Usability Questionnaire.xlsx
+++ b/F21MP/Testing/Student Testing/Survey Results/Post-Usability Questionnaire.xlsx
@@ -5,27 +5,39 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kausa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kausa\Documents\GitHub\Coursework-Wizard-Deadlines-Visualiser\F21MP\Testing\Student Testing\Survey Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0C662A-FAEA-4DDE-AF9F-EEB9B4FBCB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1762A3D8-9B7F-43CB-A48A-340092097E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -198,6 +210,94 @@
   </si>
   <si>
     <t xml:space="preserve"> 19:15:56</t>
+  </si>
+  <si>
+    <t>colour palette rating</t>
+  </si>
+  <si>
+    <t>size appropriate?</t>
+  </si>
+  <si>
+    <t>differentiate between links and content</t>
+  </si>
+  <si>
+    <t>avg:</t>
+  </si>
+  <si>
+    <t>9 Yes and 1 No</t>
+  </si>
+  <si>
+    <t>7 Yes and 3 No</t>
+  </si>
+  <si>
+    <t>major challenge</t>
+  </si>
+  <si>
+    <t>suggestion</t>
+  </si>
+  <si>
+    <t>drag</t>
+  </si>
+  <si>
+    <t>drag
+task definiton</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the overall look and UI for the website can be improved to make it look more appealing </t>
+  </si>
+  <si>
+    <t>loved the timeline and progress features!!</t>
+  </si>
+  <si>
+    <t>the sidebar (navigation bar) could be a bit smaller
+less compact
+the courses page could have the code of the courses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drag
+update your password task is a bit confusing but other than that it was good. </t>
+  </si>
+  <si>
+    <t>drag: 4</t>
+  </si>
+  <si>
+    <t>update password: 1</t>
+  </si>
+  <si>
+    <t>task definition: 1</t>
+  </si>
+  <si>
+    <t>password change in settings</t>
+  </si>
+  <si>
+    <t>more menu options</t>
+  </si>
+  <si>
+    <t>smaller side bar</t>
+  </si>
+  <si>
+    <t>add course code to all course pages</t>
+  </si>
+  <si>
+    <t>less compact (less clutter), simple dashboard by adding more pages</t>
+  </si>
+  <si>
+    <t>tutorial for beginners that don’t use canvas</t>
+  </si>
+  <si>
+    <t>instructions for drag and drop</t>
+  </si>
+  <si>
+    <t>show hide in confirm pass</t>
+  </si>
+  <si>
+    <t>consistent fonts and sizes</t>
+  </si>
+  <si>
+    <t>overall look and UI</t>
   </si>
 </sst>
 </file>
@@ -207,7 +307,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,16 +315,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -232,11 +358,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -244,6 +407,27 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,15 +858,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView topLeftCell="W1" workbookViewId="0">
+      <selection sqref="A1:W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.44140625" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" hidden="1" customWidth="1"/>
     <col min="4" max="10" width="20" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="49.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="20" hidden="1" customWidth="1"/>
@@ -1104,4 +1288,310 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD063032-3030-4B31-AA6D-7AC6C1F57E9F}">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="117.21875" customWidth="1"/>
+    <col min="6" max="6" width="96.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>8</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10">
+        <v>7</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10">
+        <v>10</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>9</v>
+      </c>
+      <c r="B9" s="10">
+        <v>4</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>10</v>
+      </c>
+      <c r="B10" s="8">
+        <v>10</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
+      <c r="B11" s="10">
+        <v>6</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="13">
+        <f>AVERAGE(B2:B11)</f>
+        <v>7.7</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F17" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F18" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F19" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F20" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F21" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F22" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F23" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>